<commit_message>
Criei o dicionário das abreviações dos medicamentos. Adicionei duas tabelas de resistencia, uma de presença e uma de prevalencia. O artigo está nas referencias. Tbm criei pastas 'out of data' para dizer que o arquivo está destualizado, mas pode conter informação importante. Preciso organiza o Home_Functions para conseguir limpar o código.
</commit_message>
<xml_diff>
--- a/Data/Modelo de Tabela.xlsx
+++ b/Data/Modelo de Tabela.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Baby Step 01" sheetId="1" r:id="rId1"/>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -838,15 +838,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="13" width="14.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Começo da refatoração do código. Criação de classes e métodos. É impossível manipular os dados do jeito que está. O código está muito confuso.
</commit_message>
<xml_diff>
--- a/Data/Modelo de Tabela.xlsx
+++ b/Data/Modelo de Tabela.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\MasterDegreeHCV\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7700"/>
   </bookViews>
   <sheets>
     <sheet name="Baby Step 01" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
   <si>
     <t>Tabela dos Pacientes</t>
   </si>
@@ -27,9 +32,6 @@
   </si>
   <si>
     <t>Baby Step 01</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>genotipo</t>
@@ -110,7 +112,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -179,6 +181,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -441,41 +446,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="2" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="1"/>
+    <col min="17" max="17" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -509,46 +514,46 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -558,7 +563,7 @@
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -566,65 +571,65 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1">
-        <v>28</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2">
-        <v>28</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" s="2">
         <v>28</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -632,62 +637,62 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="2">
         <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="2">
+        <v>28</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>28</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="2">
-        <v>28</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
-      <c r="R4" s="1">
-        <v>28</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="T4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="X4" s="1">
         <v>2.5</v>
@@ -701,13 +706,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
@@ -716,13 +721,13 @@
         <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -731,19 +736,19 @@
         <v>29</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="X5" s="1">
         <v>2.5</v>
@@ -755,13 +760,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -769,13 +774,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -783,13 +788,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -797,13 +802,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <v>92</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -811,13 +816,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1">
         <v>93</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W10" s="4"/>
     </row>
@@ -835,60 +840,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="16.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:13">

</xml_diff>